<commit_message>
fix some bug in OT Lieu data
</commit_message>
<xml_diff>
--- a/rawdata/employeelist.xlsx
+++ b/rawdata/employeelist.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Attendance-System\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1314FA98-F907-4806-A144-F2DA25BF1A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D48974E-008D-4324-90CD-42FC367554ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" xr2:uid="{D67A9D5F-8507-4763-A51C-5F8B72BE0D33}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$K$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
   <si>
     <t>STT</t>
   </si>
@@ -294,13 +294,40 @@
   </si>
   <si>
     <t>Nguyen Thi Hang6970000015</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>E&amp;S</t>
+  </si>
+  <si>
+    <t>Intern</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +345,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -340,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -358,6 +390,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,20 +733,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F25830-91F3-44EE-92C6-80AB8147A040}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="7"/>
     <col min="2" max="2" width="17.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -715,10 +762,24 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="8">
@@ -727,10 +788,22 @@
       <c r="C2" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="5">
@@ -739,10 +812,20 @@
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="8">
@@ -751,10 +834,22 @@
       <c r="C4" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="8">
@@ -763,10 +858,20 @@
       <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="5">
@@ -775,10 +880,19 @@
       <c r="C6" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="8">
@@ -787,10 +901,20 @@
       <c r="C7" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="5">
@@ -799,10 +923,20 @@
       <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="5">
@@ -811,10 +945,20 @@
       <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="8" t="e">
@@ -823,10 +967,20 @@
       <c r="C10" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="8" t="e">
@@ -835,10 +989,20 @@
       <c r="C11" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="5">
@@ -847,10 +1011,20 @@
       <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="8" t="e">
@@ -859,10 +1033,20 @@
       <c r="C13" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="8">
@@ -871,10 +1055,20 @@
       <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="5">
@@ -883,10 +1077,20 @@
       <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="8" t="e">
@@ -895,10 +1099,20 @@
       <c r="C16" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="5">
@@ -907,10 +1121,20 @@
       <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="8">
@@ -919,10 +1143,20 @@
       <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="5">
@@ -931,10 +1165,20 @@
       <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="8">
@@ -943,10 +1187,20 @@
       <c r="C20" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="5">
@@ -955,10 +1209,20 @@
       <c r="C21" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="5">
@@ -967,10 +1231,20 @@
       <c r="C22" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="8">
@@ -979,10 +1253,20 @@
       <c r="C23" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="5">
@@ -991,10 +1275,20 @@
       <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="5">
@@ -1003,10 +1297,20 @@
       <c r="C25" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="5">
@@ -1015,10 +1319,20 @@
       <c r="C26" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="5">
@@ -1027,17 +1341,24 @@
       <c r="C27" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="2"/>
+      <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16">
       <c r="A28" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="5">
@@ -1046,17 +1367,24 @@
       <c r="C28" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16">
       <c r="A29" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="8">
@@ -1065,17 +1393,24 @@
       <c r="C29" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="2"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="2"/>
+      <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16">
       <c r="A30" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="8">
@@ -1084,17 +1419,24 @@
       <c r="C30" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16">
       <c r="A31" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="8" t="e">
@@ -1103,17 +1445,24 @@
       <c r="C31" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="D31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="2"/>
+      <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16">
       <c r="A32" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="8">
@@ -1122,17 +1471,24 @@
       <c r="C32" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="D32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="2"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16">
       <c r="A33" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="8">
@@ -1141,17 +1497,24 @@
       <c r="C33" s="7" t="s">
         <v>74</v>
       </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="2"/>
+      <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16">
       <c r="A34" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A34:A65" si="1">ROW()-1</f>
         <v>33</v>
       </c>
       <c r="B34" s="8">
@@ -1160,17 +1523,24 @@
       <c r="C34" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="D34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="2"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="2"/>
+      <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16">
       <c r="A35" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="5">
@@ -1179,17 +1549,26 @@
       <c r="C35" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="D35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="4"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="2"/>
+      <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16">
       <c r="A36" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="8">
@@ -1198,17 +1577,24 @@
       <c r="C36" s="7" t="s">
         <v>48</v>
       </c>
+      <c r="D36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="2"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="2"/>
+      <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16">
       <c r="A37" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="8">
@@ -1217,17 +1603,24 @@
       <c r="C37" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="D37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="2"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16">
       <c r="A38" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="5">
@@ -1236,17 +1629,24 @@
       <c r="C38" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="D38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="2"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16">
       <c r="A39" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="8">
@@ -1255,17 +1655,24 @@
       <c r="C39" s="7" t="s">
         <v>49</v>
       </c>
+      <c r="D39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="2"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="2"/>
+      <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16">
       <c r="A40" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="5">
@@ -1274,17 +1681,24 @@
       <c r="C40" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="D40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="2"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="2"/>
+      <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16">
       <c r="A41" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="5">
@@ -1293,17 +1707,24 @@
       <c r="C41" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="D41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="2"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="2"/>
+      <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16">
       <c r="A42" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="8">
@@ -1312,17 +1733,24 @@
       <c r="C42" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="D42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="4"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="2"/>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16">
       <c r="A43" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="8" t="e">
@@ -1331,17 +1759,24 @@
       <c r="C43" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="D43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="2"/>
+      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16">
       <c r="A44" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="8">
@@ -1350,17 +1785,24 @@
       <c r="C44" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="D44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="4"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="2"/>
+      <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16">
       <c r="A45" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="8">
@@ -1369,17 +1811,24 @@
       <c r="C45" s="7" t="s">
         <v>70</v>
       </c>
+      <c r="D45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="4"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="2"/>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16">
       <c r="A46" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="8">
@@ -1388,17 +1837,24 @@
       <c r="C46" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="D46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="4"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="2"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16">
       <c r="A47" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="8">
@@ -1407,17 +1863,24 @@
       <c r="C47" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="D47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="2"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="2"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16">
       <c r="A48" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="5">
@@ -1426,17 +1889,24 @@
       <c r="C48" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="D48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="2"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="2"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16">
       <c r="A49" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="5">
@@ -1445,17 +1915,24 @@
       <c r="C49" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="D49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="2"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="2"/>
+      <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16">
       <c r="A50" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="8" t="e">
@@ -1464,17 +1941,24 @@
       <c r="C50" s="7" t="s">
         <v>77</v>
       </c>
+      <c r="D50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="2"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="2"/>
+      <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16">
       <c r="A51" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="8">
@@ -1483,17 +1967,24 @@
       <c r="C51" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="D51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="2"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="2"/>
+      <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16">
       <c r="A52" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" s="8">
@@ -1502,17 +1993,24 @@
       <c r="C52" s="7" t="s">
         <v>72</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="2"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="2"/>
+      <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16">
       <c r="A53" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="5">
@@ -1521,17 +2019,24 @@
       <c r="C53" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="2"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16">
       <c r="A54" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="5">
@@ -1540,17 +2045,24 @@
       <c r="C54" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="D54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="2"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="2"/>
+      <c r="K54" s="3"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="3"/>
       <c r="P54" s="3"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16">
       <c r="A55" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="5">
@@ -1559,17 +2071,26 @@
       <c r="C55" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="D55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="2"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="2"/>
+      <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16">
       <c r="A56" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="5">
@@ -1578,17 +2099,24 @@
       <c r="C56" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="D56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="2"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="2"/>
+      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16">
       <c r="A57" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="8">
@@ -1597,17 +2125,26 @@
       <c r="C57" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="D57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="2"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="4"/>
+      <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="3"/>
       <c r="P57" s="3"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16">
       <c r="A58" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="8" t="e">
@@ -1616,17 +2153,24 @@
       <c r="C58" s="7" t="s">
         <v>78</v>
       </c>
+      <c r="D58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="2"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="4"/>
+      <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16">
       <c r="A59" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="5">
@@ -1635,17 +2179,24 @@
       <c r="C59" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="D59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="2"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="2"/>
+      <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16">
       <c r="A60" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="8">
@@ -1654,17 +2205,24 @@
       <c r="C60" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="D60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="2"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="2"/>
+      <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16">
       <c r="A61" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" s="5">
@@ -1673,17 +2231,24 @@
       <c r="C61" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="2"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="2"/>
+      <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16">
       <c r="A62" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" s="5">
@@ -1692,17 +2257,24 @@
       <c r="C62" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="D62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="2"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="2"/>
+      <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16">
       <c r="A63" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" s="8">
@@ -1711,17 +2283,24 @@
       <c r="C63" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="D63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="2"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="4"/>
+      <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16">
       <c r="A64" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" s="8" t="e">
@@ -1730,17 +2309,24 @@
       <c r="C64" s="7" t="s">
         <v>79</v>
       </c>
+      <c r="D64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="2"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
-      <c r="K64" s="4"/>
+      <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16">
       <c r="A65" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B65" s="5">
@@ -1749,17 +2335,24 @@
       <c r="C65" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="D65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="2"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
-      <c r="K65" s="4"/>
+      <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16">
       <c r="A66" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A66:A83" si="2">ROW()-1</f>
         <v>65</v>
       </c>
       <c r="B66" s="5">
@@ -1768,17 +2361,24 @@
       <c r="C66" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="D66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="2"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="4"/>
+      <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16">
       <c r="A67" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="B67" s="8">
@@ -1787,17 +2387,24 @@
       <c r="C67" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="D67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="2"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
-      <c r="K67" s="4"/>
+      <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16">
       <c r="A68" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="B68" s="8">
@@ -1806,17 +2413,24 @@
       <c r="C68" s="7" t="s">
         <v>71</v>
       </c>
+      <c r="D68" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="4"/>
       <c r="I68" s="1"/>
-      <c r="J68" s="2"/>
+      <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16">
       <c r="A69" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="B69" s="8">
@@ -1825,17 +2439,24 @@
       <c r="C69" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="D69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="2"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
-      <c r="K69" s="2"/>
+      <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16">
       <c r="A70" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="B70" s="8">
@@ -1844,17 +2465,24 @@
       <c r="C70" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="D70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="2"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
-      <c r="K70" s="2"/>
+      <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16">
       <c r="A71" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B71" s="5">
@@ -1863,17 +2491,24 @@
       <c r="C71" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="D71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="2"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
-      <c r="K71" s="2"/>
+      <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16">
       <c r="A72" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="B72" s="5">
@@ -1882,17 +2517,24 @@
       <c r="C72" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="D72" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="4"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
-      <c r="K72" s="2"/>
+      <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16">
       <c r="A73" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="B73" s="5">
@@ -1901,17 +2543,24 @@
       <c r="C73" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="D73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="2"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
-      <c r="K73" s="4"/>
+      <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16">
       <c r="A74" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="B74" s="5">
@@ -1920,17 +2569,24 @@
       <c r="C74" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="D74" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="4"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
-      <c r="K74" s="2"/>
+      <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16">
       <c r="A75" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="B75" s="8">
@@ -1939,17 +2595,24 @@
       <c r="C75" s="7" t="s">
         <v>66</v>
       </c>
+      <c r="D75" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="4"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
-      <c r="K75" s="2"/>
+      <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16">
       <c r="A76" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B76" s="5">
@@ -1958,17 +2621,24 @@
       <c r="C76" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="2"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
-      <c r="K76" s="2"/>
+      <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16">
       <c r="A77" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="B77" s="8">
@@ -1977,17 +2647,24 @@
       <c r="C77" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="D77" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="2"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
-      <c r="K77" s="2"/>
+      <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="P77" s="1"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16">
       <c r="A78" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="B78" s="5">
@@ -1996,17 +2673,24 @@
       <c r="C78" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="D78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="2"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
-      <c r="K78" s="2"/>
+      <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16">
       <c r="A79" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B79" s="8">
@@ -2015,17 +2699,24 @@
       <c r="C79" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="D79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="4"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="2"/>
+      <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="P79" s="1"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16">
       <c r="A80" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="B80" s="5">
@@ -2034,17 +2725,24 @@
       <c r="C80" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="D80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="2"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80" s="2"/>
+      <c r="K80" s="3"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="P80" s="1"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16">
       <c r="A81" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="B81" s="8">
@@ -2053,6 +2751,10 @@
       <c r="C81" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="D81" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="2"/>
@@ -2061,9 +2763,9 @@
       <c r="N81" s="1"/>
       <c r="P81" s="1"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16">
       <c r="A82" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="B82" s="8">
@@ -2072,6 +2774,10 @@
       <c r="C82" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="D82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="2"/>
@@ -2080,9 +2786,9 @@
       <c r="N82" s="1"/>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16">
       <c r="A83" s="7">
-        <f>ROW()-1</f>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="B83" s="8">
@@ -2090,6 +2796,12 @@
       </c>
       <c r="C83" s="7" t="s">
         <v>55</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>

</xml_diff>